<commit_message>
add 24 med/biorxiv images to COVID data
</commit_message>
<xml_diff>
--- a/COVID-CT-MetaInfo.xlsx
+++ b/COVID-CT-MetaInfo.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28908"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yichenzhang/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fischer/UCSD/XPT's Lab/COVID-CT/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4799F844-5A7C-B441-82EB-C7A287E28F93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="positive_captions" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="560">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="597">
   <si>
     <t>2020.03.01.20029769-p21-73_1%1.png</t>
   </si>
@@ -1707,31 +1708,192 @@
   </si>
   <si>
     <t>Patient 169</t>
+  </si>
+  <si>
+    <t>['Figure 1 Various chest CT imaging features of COVID-19 GGO, ground glass opacity ']</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Figure S1. Representative dynamic changes in chest computer tomography (CT) scans from two patients with COVID-19. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="CIDFont+F1"/>
+      </rPr>
+      <t xml:space="preserve">A1–A3, CT images of a 70- year-old male patient, who progressed from the non-severe to critical disease group, and died. A1 (day 1), A2 (day 4), A3 (day 9): below the pleura are scattered shadows of frosted glass, large sheet diffuse paving stones in both lungs, and extensive consolidation of both lungs with thickening of interlobular stroma repetitively. B1–B3, CT images of a 44-year-old female patient, who progressed from the critical to non-severe disease group. B1 (day 3) exhibiting extensive consolidation of both lungs; B2 (day 9) exhibiting frosted hyaline change and paving stone signs. B3 (day 20) showing significant resolution of ground-glass opacities and subpleural cord changes. </t>
+    </r>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>2020.03.25.20037721-p27-165.png</t>
+  </si>
+  <si>
+    <t>2020.03.25.20037721-p27-172.png</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>2020.03.25.20037721-p27-173.png</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>2020.03.25.20037721-p27-174.png</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>2020.03.25.20037721-p27-181.png</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>2020.03.25.20037721-p27-182.png</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>Patient 170</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>Patient 171</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>2020.03.25.20043166-p17-78</t>
+  </si>
+  <si>
+    <t>Patient 172</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>Patient 173</t>
+  </si>
+  <si>
+    <t>Patient 174</t>
+  </si>
+  <si>
+    <t>Patient 175</t>
+  </si>
+  <si>
+    <t>2020.03.25.20043166-p17-79</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>2020.03.25.20043166-p17-80</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>2020.03.25.20043166-p17-81</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">CT scan of the four cases </t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>2020.03.26.20041426-p11-119</t>
+  </si>
+  <si>
+    <t>2020.03.26.20041426-p11-120</t>
+  </si>
+  <si>
+    <t>2020.03.26.20041426-p11-121</t>
+  </si>
+  <si>
+    <t>2020.03.26.20041426-p11-122</t>
+  </si>
+  <si>
+    <t>2020.03.26.20041426-p11-123</t>
+  </si>
+  <si>
+    <t>2020.03.26.20041426-p11-124</t>
+  </si>
+  <si>
+    <t>2020.03.26.20041426-p11-125</t>
+  </si>
+  <si>
+    <t>2020.03.26.20041426-p11-126</t>
+  </si>
+  <si>
+    <t>Patient 176</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Fig2. Chest CT images of a 26-year-old patient with COVID-19. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">a Chest CT images obtained on February 2, 2020, showed ground glass opacity in both lungs on day 5 after symptom onset. b Images taken on February 12,2020, indicated the lesions increased obviously. C Images taken on February 19, 2020.revealed bilateral ground glass opacity absorbed dramatically, and the patient discharged from hospital and return to the local hospital. </t>
+    </r>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>2020.03.26.20041426-p11-127</t>
+  </si>
+  <si>
+    <t>2020.03.26.20041426-p11-128</t>
+  </si>
+  <si>
+    <t>2020.03.26.20041426-p11-130</t>
+  </si>
+  <si>
+    <t>2020.03.26.20041426-p11-131</t>
+  </si>
+  <si>
+    <t>2020.03.26.20041426-p11-132</t>
+  </si>
+  <si>
+    <t>2020.03.26.20041426-p11-133</t>
+  </si>
+  <si>
+    <t>Patient 177</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Fig3. Chest CT images of a 62-year-old patient with COVID-19. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">a Chest CT images obtained on February 2, 2020, showed ground glass opacity in both lungs on day 5 after symptom onset. b Images taken on February 11,2020, revealed the lesions increased rapidly, and the patient died on February 16,2020. </t>
+    </r>
+    <phoneticPr fontId="19" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="Calibri Light"/>
+      <name val="等线 Light"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
@@ -1739,7 +1901,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1747,7 +1909,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1755,35 +1917,35 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1791,7 +1953,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1799,14 +1961,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1814,14 +1976,14 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1829,7 +1991,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1837,16 +1999,34 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="CIDFont+F1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="33">
@@ -2194,48 +2374,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="标题" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="标题 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="标题 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="标题 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="标题 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="差" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="好" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="汇总" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="计算" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="检查单元格" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="解释性文本" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="警告文本" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="链接单元格" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="适中" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="输出" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="输入" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="着色 1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="着色 2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="着色 3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="着色 4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="着色 5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2546,20 +2726,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C264"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C288"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A260" workbookViewId="0">
+      <selection activeCell="A288" sqref="A288"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="161.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>222</v>
       </c>
@@ -2570,7 +2750,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>228</v>
       </c>
@@ -2581,7 +2761,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>186</v>
       </c>
@@ -2592,7 +2772,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>193</v>
       </c>
@@ -2603,7 +2783,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>219</v>
       </c>
@@ -2614,7 +2794,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>234</v>
       </c>
@@ -2625,7 +2805,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>250</v>
       </c>
@@ -2636,7 +2816,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>249</v>
       </c>
@@ -2647,7 +2827,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>225</v>
       </c>
@@ -2658,7 +2838,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>226</v>
       </c>
@@ -2669,7 +2849,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>189</v>
       </c>
@@ -2680,7 +2860,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>190</v>
       </c>
@@ -2691,7 +2871,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>257</v>
       </c>
@@ -2702,7 +2882,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
         <v>241</v>
       </c>
@@ -2713,7 +2893,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>211</v>
       </c>
@@ -2724,7 +2904,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
         <v>199</v>
       </c>
@@ -2735,7 +2915,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>183</v>
       </c>
@@ -2746,7 +2926,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>196</v>
       </c>
@@ -2757,7 +2937,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>48</v>
       </c>
@@ -2768,7 +2948,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -2779,7 +2959,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>75</v>
       </c>
@@ -2790,7 +2970,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>62</v>
       </c>
@@ -2801,7 +2981,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>79</v>
       </c>
@@ -2812,7 +2992,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>142</v>
       </c>
@@ -2823,7 +3003,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>150</v>
       </c>
@@ -2834,7 +3014,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3">
       <c r="A26" t="s">
         <v>172</v>
       </c>
@@ -2845,7 +3025,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3">
       <c r="A27" t="s">
         <v>164</v>
       </c>
@@ -2856,7 +3036,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3">
       <c r="A28" t="s">
         <v>217</v>
       </c>
@@ -2867,7 +3047,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3">
       <c r="A29" t="s">
         <v>235</v>
       </c>
@@ -2878,7 +3058,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3">
       <c r="A30" t="s">
         <v>259</v>
       </c>
@@ -2889,7 +3069,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3">
       <c r="A31" t="s">
         <v>46</v>
       </c>
@@ -2900,7 +3080,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3">
       <c r="A32" t="s">
         <v>39</v>
       </c>
@@ -2911,7 +3091,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3">
       <c r="A33" t="s">
         <v>52</v>
       </c>
@@ -2922,7 +3102,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3">
       <c r="A34" t="s">
         <v>59</v>
       </c>
@@ -2933,7 +3113,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3">
       <c r="A35" t="s">
         <v>23</v>
       </c>
@@ -2944,7 +3124,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3">
       <c r="A36" t="s">
         <v>89</v>
       </c>
@@ -2955,7 +3135,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3">
       <c r="A37" t="s">
         <v>82</v>
       </c>
@@ -2966,7 +3146,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3">
       <c r="A38" t="s">
         <v>64</v>
       </c>
@@ -2977,7 +3157,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3">
       <c r="A39" t="s">
         <v>73</v>
       </c>
@@ -2988,7 +3168,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3">
       <c r="A40" t="s">
         <v>247</v>
       </c>
@@ -2999,7 +3179,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3">
       <c r="A41" t="s">
         <v>253</v>
       </c>
@@ -3010,7 +3190,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3">
       <c r="A42" t="s">
         <v>229</v>
       </c>
@@ -3021,7 +3201,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3">
       <c r="A43" t="s">
         <v>25</v>
       </c>
@@ -3032,7 +3212,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3">
       <c r="A44" t="s">
         <v>30</v>
       </c>
@@ -3043,7 +3223,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3">
       <c r="A45" t="s">
         <v>12</v>
       </c>
@@ -3054,7 +3234,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3">
       <c r="A46" t="s">
         <v>7</v>
       </c>
@@ -3065,7 +3245,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3">
       <c r="A47" t="s">
         <v>43</v>
       </c>
@@ -3076,7 +3256,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3">
       <c r="A48" t="s">
         <v>42</v>
       </c>
@@ -3087,7 +3267,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3">
       <c r="A49" t="s">
         <v>35</v>
       </c>
@@ -3098,7 +3278,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3">
       <c r="A50" t="s">
         <v>50</v>
       </c>
@@ -3109,7 +3289,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3">
       <c r="A51" t="s">
         <v>60</v>
       </c>
@@ -3120,7 +3300,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -3131,7 +3311,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3">
       <c r="A53" t="s">
         <v>177</v>
       </c>
@@ -3142,7 +3322,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3">
       <c r="A54" t="s">
         <v>160</v>
       </c>
@@ -3153,7 +3333,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3">
       <c r="A55" t="s">
         <v>139</v>
       </c>
@@ -3164,7 +3344,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3">
       <c r="A56" t="s">
         <v>154</v>
       </c>
@@ -3175,7 +3355,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3">
       <c r="A57" t="s">
         <v>113</v>
       </c>
@@ -3186,7 +3366,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3">
       <c r="A58" t="s">
         <v>124</v>
       </c>
@@ -3197,7 +3377,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3">
       <c r="A59" t="s">
         <v>90</v>
       </c>
@@ -3208,7 +3388,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3">
       <c r="A60" t="s">
         <v>81</v>
       </c>
@@ -3219,7 +3399,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3">
       <c r="A61" t="s">
         <v>65</v>
       </c>
@@ -3230,7 +3410,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:3">
       <c r="A62" t="s">
         <v>72</v>
       </c>
@@ -3241,7 +3421,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:3">
       <c r="A63" t="s">
         <v>69</v>
       </c>
@@ -3252,7 +3432,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:3">
       <c r="A64" t="s">
         <v>168</v>
       </c>
@@ -3263,7 +3443,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:3">
       <c r="A65" t="s">
         <v>147</v>
       </c>
@@ -3274,7 +3454,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:3">
       <c r="A66" t="s">
         <v>145</v>
       </c>
@@ -3285,7 +3465,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:3">
       <c r="A67" t="s">
         <v>221</v>
       </c>
@@ -3296,7 +3476,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:3">
       <c r="A68" t="s">
         <v>231</v>
       </c>
@@ -3307,7 +3487,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:3">
       <c r="A69" t="s">
         <v>256</v>
       </c>
@@ -3318,7 +3498,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:3">
       <c r="A70" t="s">
         <v>243</v>
       </c>
@@ -3329,7 +3509,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:3">
       <c r="A71" t="s">
         <v>210</v>
       </c>
@@ -3340,7 +3520,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:3">
       <c r="A72" t="s">
         <v>201</v>
       </c>
@@ -3351,7 +3531,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:3">
       <c r="A73" t="s">
         <v>167</v>
       </c>
@@ -3362,7 +3542,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:3">
       <c r="A74" t="s">
         <v>169</v>
       </c>
@@ -3373,7 +3553,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:3">
       <c r="A75" t="s">
         <v>129</v>
       </c>
@@ -3384,7 +3564,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:3">
       <c r="A76" t="s">
         <v>133</v>
       </c>
@@ -3395,7 +3575,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:3">
       <c r="A77" t="s">
         <v>119</v>
       </c>
@@ -3406,7 +3586,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:3">
       <c r="A78" t="s">
         <v>118</v>
       </c>
@@ -3417,7 +3597,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:3">
       <c r="A79" t="s">
         <v>97</v>
       </c>
@@ -3428,7 +3608,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:3">
       <c r="A80" t="s">
         <v>101</v>
       </c>
@@ -3439,7 +3619,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:3">
       <c r="A81" t="s">
         <v>195</v>
       </c>
@@ -3450,7 +3630,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:3">
       <c r="A82" t="s">
         <v>182</v>
       </c>
@@ -3461,7 +3641,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:3">
       <c r="A83" t="s">
         <v>200</v>
       </c>
@@ -3472,7 +3652,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:3">
       <c r="A84" t="s">
         <v>212</v>
       </c>
@@ -3483,7 +3663,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:3">
       <c r="A85" t="s">
         <v>242</v>
       </c>
@@ -3494,7 +3674,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:3">
       <c r="A86" t="s">
         <v>258</v>
       </c>
@@ -3505,7 +3685,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:3">
       <c r="A87" t="s">
         <v>233</v>
       </c>
@@ -3516,7 +3696,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:3">
       <c r="A88" t="s">
         <v>218</v>
       </c>
@@ -3527,7 +3707,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:3">
       <c r="A89" t="s">
         <v>3</v>
       </c>
@@ -3538,7 +3718,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:3">
       <c r="A90" t="s">
         <v>16</v>
       </c>
@@ -3549,7 +3729,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:3">
       <c r="A91" t="s">
         <v>216</v>
       </c>
@@ -3560,7 +3740,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:3">
       <c r="A92" t="s">
         <v>236</v>
       </c>
@@ -3571,7 +3751,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:3">
       <c r="A93" t="s">
         <v>53</v>
       </c>
@@ -3582,7 +3762,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:3">
       <c r="A94" t="s">
         <v>58</v>
       </c>
@@ -3593,7 +3773,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:3">
       <c r="A95" t="s">
         <v>111</v>
       </c>
@@ -3604,7 +3784,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:3">
       <c r="A96" t="s">
         <v>104</v>
       </c>
@@ -3615,7 +3795,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:3">
       <c r="A97" t="s">
         <v>91</v>
       </c>
@@ -3626,7 +3806,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:3">
       <c r="A98" t="s">
         <v>80</v>
       </c>
@@ -3637,7 +3817,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:3">
       <c r="A99" t="s">
         <v>21</v>
       </c>
@@ -3648,7 +3828,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:3">
       <c r="A100" t="s">
         <v>34</v>
       </c>
@@ -3659,7 +3839,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:3">
       <c r="A101" t="s">
         <v>67</v>
       </c>
@@ -3670,7 +3850,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:3">
       <c r="A102" t="s">
         <v>70</v>
       </c>
@@ -3681,7 +3861,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:3">
       <c r="A103" t="s">
         <v>143</v>
       </c>
@@ -3692,7 +3872,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:3">
       <c r="A104" t="s">
         <v>148</v>
       </c>
@@ -3703,7 +3883,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:3">
       <c r="A105" t="s">
         <v>171</v>
       </c>
@@ -3714,7 +3894,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:3">
       <c r="A106" t="s">
         <v>165</v>
       </c>
@@ -3725,7 +3905,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:3">
       <c r="A107" t="s">
         <v>131</v>
       </c>
@@ -3736,7 +3916,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:3">
       <c r="A108" t="s">
         <v>157</v>
       </c>
@@ -3747,7 +3927,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:3">
       <c r="A109" t="s">
         <v>179</v>
       </c>
@@ -3758,7 +3938,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:3">
       <c r="A110" t="s">
         <v>19</v>
       </c>
@@ -3769,7 +3949,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:3">
       <c r="A111" t="s">
         <v>0</v>
       </c>
@@ -3780,7 +3960,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:3">
       <c r="A112" t="s">
         <v>20</v>
       </c>
@@ -3791,7 +3971,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:3">
       <c r="A113" t="s">
         <v>63</v>
       </c>
@@ -3802,7 +3982,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:3">
       <c r="A114" t="s">
         <v>74</v>
       </c>
@@ -3813,7 +3993,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:3">
       <c r="A115" t="s">
         <v>92</v>
       </c>
@@ -3824,7 +4004,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:3">
       <c r="A116" t="s">
         <v>112</v>
       </c>
@@ -3835,7 +4015,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:3">
       <c r="A117" t="s">
         <v>78</v>
       </c>
@@ -3846,7 +4026,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:3">
       <c r="A118" t="s">
         <v>158</v>
       </c>
@@ -3857,7 +4037,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:3">
       <c r="A119" t="s">
         <v>178</v>
       </c>
@@ -3868,7 +4048,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:3">
       <c r="A120" t="s">
         <v>156</v>
       </c>
@@ -3879,7 +4059,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:3">
       <c r="A121" t="s">
         <v>18</v>
       </c>
@@ -3890,7 +4070,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:3">
       <c r="A122" t="s">
         <v>1</v>
       </c>
@@ -3901,7 +4081,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:3">
       <c r="A123" t="s">
         <v>191</v>
       </c>
@@ -3912,7 +4092,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:3">
       <c r="A124" t="s">
         <v>187</v>
       </c>
@@ -3923,7 +4103,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:3">
       <c r="A125" t="s">
         <v>128</v>
       </c>
@@ -3934,7 +4114,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:3">
       <c r="A126" t="s">
         <v>134</v>
       </c>
@@ -3945,7 +4125,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:3">
       <c r="A127" t="s">
         <v>232</v>
       </c>
@@ -3956,7 +4136,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:3">
       <c r="A128" t="s">
         <v>103</v>
       </c>
@@ -3967,7 +4147,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:3">
       <c r="A129" t="s">
         <v>95</v>
       </c>
@@ -3978,7 +4158,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:3">
       <c r="A130" t="s">
         <v>197</v>
       </c>
@@ -3989,7 +4169,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:3">
       <c r="A131" t="s">
         <v>180</v>
       </c>
@@ -4000,7 +4180,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:3">
       <c r="A132" t="s">
         <v>198</v>
       </c>
@@ -4011,7 +4191,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:3">
       <c r="A133" t="s">
         <v>213</v>
       </c>
@@ -4022,7 +4202,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:3">
       <c r="A134" t="s">
         <v>239</v>
       </c>
@@ -4033,7 +4213,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:3">
       <c r="A135" t="s">
         <v>260</v>
       </c>
@@ -4044,7 +4224,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:3">
       <c r="A136" t="s">
         <v>45</v>
       </c>
@@ -4055,7 +4235,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:3">
       <c r="A137" t="s">
         <v>40</v>
       </c>
@@ -4066,7 +4246,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:3">
       <c r="A138" t="s">
         <v>54</v>
       </c>
@@ -4077,7 +4257,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:3">
       <c r="A139" t="s">
         <v>57</v>
       </c>
@@ -4088,7 +4268,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:3">
       <c r="A140" t="s">
         <v>24</v>
       </c>
@@ -4099,7 +4279,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:3">
       <c r="A141" t="s">
         <v>31</v>
       </c>
@@ -4110,7 +4290,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:3">
       <c r="A142" t="s">
         <v>13</v>
       </c>
@@ -4121,7 +4301,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:3">
       <c r="A143" t="s">
         <v>6</v>
       </c>
@@ -4132,7 +4312,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:3">
       <c r="A144" t="s">
         <v>223</v>
       </c>
@@ -4143,7 +4323,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:3">
       <c r="A145" t="s">
         <v>261</v>
       </c>
@@ -4154,7 +4334,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:3">
       <c r="A146" t="s">
         <v>238</v>
       </c>
@@ -4165,7 +4345,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:3">
       <c r="A147" t="s">
         <v>214</v>
       </c>
@@ -4176,7 +4356,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:3">
       <c r="A148" t="s">
         <v>161</v>
       </c>
@@ -4187,7 +4367,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:3">
       <c r="A149" t="s">
         <v>176</v>
       </c>
@@ -4198,7 +4378,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:3">
       <c r="A150" t="s">
         <v>153</v>
       </c>
@@ -4209,7 +4389,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:3">
       <c r="A151" t="s">
         <v>140</v>
       </c>
@@ -4220,7 +4400,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:3">
       <c r="A152" t="s">
         <v>152</v>
       </c>
@@ -4231,7 +4411,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:3">
       <c r="A153" t="s">
         <v>175</v>
       </c>
@@ -4242,7 +4422,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:3">
       <c r="A154" t="s">
         <v>162</v>
       </c>
@@ -4253,7 +4433,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:3">
       <c r="A155" t="s">
         <v>192</v>
       </c>
@@ -4264,7 +4444,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:3">
       <c r="A156" t="s">
         <v>188</v>
       </c>
@@ -4275,7 +4455,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:3">
       <c r="A157" t="s">
         <v>204</v>
       </c>
@@ -4286,7 +4466,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:3">
       <c r="A158" t="s">
         <v>207</v>
       </c>
@@ -4297,7 +4477,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:3">
       <c r="A159" t="s">
         <v>246</v>
       </c>
@@ -4308,7 +4488,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:3">
       <c r="A160" t="s">
         <v>252</v>
       </c>
@@ -4319,7 +4499,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:3">
       <c r="A161" t="s">
         <v>215</v>
       </c>
@@ -4330,7 +4510,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:3">
       <c r="A162" t="s">
         <v>237</v>
       </c>
@@ -4341,7 +4521,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:3">
       <c r="A163" t="s">
         <v>28</v>
       </c>
@@ -4352,7 +4532,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:3">
       <c r="A164" t="s">
         <v>27</v>
       </c>
@@ -4363,7 +4543,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:3">
       <c r="A165" t="s">
         <v>8</v>
       </c>
@@ -4374,7 +4554,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:3">
       <c r="A166" t="s">
         <v>11</v>
       </c>
@@ -4385,7 +4565,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:3">
       <c r="A167" t="s">
         <v>132</v>
       </c>
@@ -4396,7 +4576,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:3">
       <c r="A168" t="s">
         <v>166</v>
       </c>
@@ -4407,7 +4587,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:3">
       <c r="A169" t="s">
         <v>170</v>
       </c>
@@ -4418,7 +4598,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:3">
       <c r="A170" t="s">
         <v>149</v>
       </c>
@@ -4429,7 +4609,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:3">
       <c r="A171" t="s">
         <v>9</v>
       </c>
@@ -4440,7 +4620,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:3">
       <c r="A172" t="s">
         <v>10</v>
       </c>
@@ -4451,7 +4631,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:3">
       <c r="A173" t="s">
         <v>29</v>
       </c>
@@ -4462,7 +4642,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:3">
       <c r="A174" t="s">
         <v>26</v>
       </c>
@@ -4473,7 +4653,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:3">
       <c r="A175" t="s">
         <v>125</v>
       </c>
@@ -4484,7 +4664,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:3">
       <c r="A176" t="s">
         <v>136</v>
       </c>
@@ -4495,7 +4675,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:3">
       <c r="A177" t="s">
         <v>209</v>
       </c>
@@ -4506,7 +4686,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:3">
       <c r="A178" t="s">
         <v>202</v>
       </c>
@@ -4517,7 +4697,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:3">
       <c r="A179" t="s">
         <v>123</v>
       </c>
@@ -4528,7 +4708,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:3">
       <c r="A180" t="s">
         <v>115</v>
       </c>
@@ -4539,7 +4719,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:3">
       <c r="A181" t="s">
         <v>126</v>
       </c>
@@ -4550,7 +4730,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:3">
       <c r="A182" t="s">
         <v>135</v>
       </c>
@@ -4561,7 +4741,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:3">
       <c r="A183" t="s">
         <v>163</v>
       </c>
@@ -4572,7 +4752,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:3">
       <c r="A184" t="s">
         <v>173</v>
       </c>
@@ -4583,7 +4763,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:3">
       <c r="A185" t="s">
         <v>49</v>
       </c>
@@ -4594,7 +4774,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:3">
       <c r="A186" t="s">
         <v>36</v>
       </c>
@@ -4605,7 +4785,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:3">
       <c r="A187" t="s">
         <v>181</v>
       </c>
@@ -4616,7 +4796,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:3">
       <c r="A188" t="s">
         <v>240</v>
       </c>
@@ -4627,7 +4807,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:3">
       <c r="A189" t="s">
         <v>47</v>
       </c>
@@ -4638,7 +4818,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:3">
       <c r="A190" t="s">
         <v>2</v>
       </c>
@@ -4649,7 +4829,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:3">
       <c r="A191" t="s">
         <v>17</v>
       </c>
@@ -4660,7 +4840,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:3">
       <c r="A192" t="s">
         <v>33</v>
       </c>
@@ -4671,7 +4851,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:3">
       <c r="A193" t="s">
         <v>14</v>
       </c>
@@ -4682,7 +4862,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:3">
       <c r="A194" t="s">
         <v>4</v>
       </c>
@@ -4693,7 +4873,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:3">
       <c r="A195" t="s">
         <v>44</v>
       </c>
@@ -4704,7 +4884,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:3">
       <c r="A196" t="s">
         <v>41</v>
       </c>
@@ -4715,7 +4895,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:3">
       <c r="A197" t="s">
         <v>55</v>
       </c>
@@ -4726,7 +4906,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:3">
       <c r="A198" t="s">
         <v>56</v>
       </c>
@@ -4737,7 +4917,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:3">
       <c r="A199" t="s">
         <v>206</v>
       </c>
@@ -4748,7 +4928,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:3">
       <c r="A200" t="s">
         <v>205</v>
       </c>
@@ -4759,7 +4939,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:3">
       <c r="A201" t="s">
         <v>224</v>
       </c>
@@ -4770,7 +4950,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:3">
       <c r="A202" t="s">
         <v>227</v>
       </c>
@@ -4781,7 +4961,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:3">
       <c r="A203" t="s">
         <v>251</v>
       </c>
@@ -4792,7 +4972,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:3">
       <c r="A204" t="s">
         <v>248</v>
       </c>
@@ -4803,7 +4983,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:3">
       <c r="A205" t="s">
         <v>159</v>
       </c>
@@ -4814,7 +4994,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:3">
       <c r="A206" t="s">
         <v>138</v>
       </c>
@@ -4825,7 +5005,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:3">
       <c r="A207" t="s">
         <v>155</v>
       </c>
@@ -4836,7 +5016,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:3">
       <c r="A208" t="s">
         <v>114</v>
       </c>
@@ -4847,7 +5027,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:3">
       <c r="A209" t="s">
         <v>94</v>
       </c>
@@ -4858,7 +5038,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:3">
       <c r="A210" t="s">
         <v>77</v>
       </c>
@@ -4869,7 +5049,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:3">
       <c r="A211" t="s">
         <v>61</v>
       </c>
@@ -4880,7 +5060,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:3">
       <c r="A212" t="s">
         <v>102</v>
       </c>
@@ -4891,7 +5071,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:3">
       <c r="A213" t="s">
         <v>185</v>
       </c>
@@ -4902,7 +5082,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:3">
       <c r="A214" t="s">
         <v>203</v>
       </c>
@@ -4913,7 +5093,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:3">
       <c r="A215" t="s">
         <v>208</v>
       </c>
@@ -4924,7 +5104,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:3">
       <c r="A216" t="s">
         <v>245</v>
       </c>
@@ -4935,7 +5115,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:3">
       <c r="A217" t="s">
         <v>254</v>
       </c>
@@ -4946,7 +5126,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:3">
       <c r="A218" t="s">
         <v>230</v>
       </c>
@@ -4957,7 +5137,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:3">
       <c r="A219" t="s">
         <v>99</v>
       </c>
@@ -4968,7 +5148,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:3">
       <c r="A220" t="s">
         <v>108</v>
       </c>
@@ -4979,7 +5159,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:3">
       <c r="A221" t="s">
         <v>107</v>
       </c>
@@ -4990,7 +5170,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:3">
       <c r="A222" t="s">
         <v>86</v>
       </c>
@@ -5001,7 +5181,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:3">
       <c r="A223" t="s">
         <v>85</v>
       </c>
@@ -5012,7 +5192,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:3">
       <c r="A224" t="s">
         <v>68</v>
       </c>
@@ -5023,7 +5203,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:3">
       <c r="A225" t="s">
         <v>38</v>
       </c>
@@ -5034,7 +5214,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:3">
       <c r="A226" t="s">
         <v>184</v>
       </c>
@@ -5045,7 +5225,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:3">
       <c r="A227" t="s">
         <v>194</v>
       </c>
@@ -5056,7 +5236,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:3">
       <c r="A228" t="s">
         <v>255</v>
       </c>
@@ -5067,7 +5247,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:3">
       <c r="A229" t="s">
         <v>244</v>
       </c>
@@ -5078,7 +5258,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:3">
       <c r="A230" t="s">
         <v>220</v>
       </c>
@@ -5089,7 +5269,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:3">
       <c r="A231" t="s">
         <v>130</v>
       </c>
@@ -5100,7 +5280,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:3">
       <c r="A232" t="s">
         <v>117</v>
       </c>
@@ -5111,7 +5291,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:3">
       <c r="A233" t="s">
         <v>121</v>
       </c>
@@ -5122,7 +5302,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:3">
       <c r="A234" t="s">
         <v>146</v>
       </c>
@@ -5133,7 +5313,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:3">
       <c r="A235" t="s">
         <v>5</v>
       </c>
@@ -5144,7 +5324,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:3">
       <c r="A236" t="s">
         <v>98</v>
       </c>
@@ -5155,7 +5335,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:3">
       <c r="A237" t="s">
         <v>106</v>
       </c>
@@ -5166,7 +5346,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:3">
       <c r="A238" t="s">
         <v>109</v>
       </c>
@@ -5177,7 +5357,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:3">
       <c r="A239" t="s">
         <v>83</v>
       </c>
@@ -5188,7 +5368,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:3">
       <c r="A240" t="s">
         <v>88</v>
       </c>
@@ -5199,7 +5379,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:3">
       <c r="A241" t="s">
         <v>66</v>
       </c>
@@ -5210,7 +5390,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:3">
       <c r="A242" t="s">
         <v>144</v>
       </c>
@@ -5221,7 +5401,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:3">
       <c r="A243" t="s">
         <v>137</v>
       </c>
@@ -5232,7 +5412,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:3">
       <c r="A244" t="s">
         <v>76</v>
       </c>
@@ -5243,7 +5423,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:3">
       <c r="A245" t="s">
         <v>93</v>
       </c>
@@ -5254,7 +5434,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:3">
       <c r="A246" t="s">
         <v>15</v>
       </c>
@@ -5265,7 +5445,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:3">
       <c r="A247" t="s">
         <v>32</v>
       </c>
@@ -5276,7 +5456,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:3">
       <c r="A248" t="s">
         <v>22</v>
       </c>
@@ -5287,7 +5467,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:3">
       <c r="A249" t="s">
         <v>71</v>
       </c>
@@ -5298,7 +5478,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:3">
       <c r="A250" t="s">
         <v>87</v>
       </c>
@@ -5309,7 +5489,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:3">
       <c r="A251" t="s">
         <v>84</v>
       </c>
@@ -5320,7 +5500,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:3">
       <c r="A252" t="s">
         <v>110</v>
       </c>
@@ -5331,7 +5511,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:3">
       <c r="A253" t="s">
         <v>105</v>
       </c>
@@ -5342,7 +5522,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:3">
       <c r="A254" t="s">
         <v>96</v>
       </c>
@@ -5353,7 +5533,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:3">
       <c r="A255" t="s">
         <v>100</v>
       </c>
@@ -5364,7 +5544,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:3">
       <c r="A256" t="s">
         <v>120</v>
       </c>
@@ -5375,7 +5555,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:3">
       <c r="A257" t="s">
         <v>174</v>
       </c>
@@ -5386,7 +5566,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:3">
       <c r="A258" t="s">
         <v>151</v>
       </c>
@@ -5397,7 +5577,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:3">
       <c r="A259" t="s">
         <v>141</v>
       </c>
@@ -5408,7 +5588,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:3">
       <c r="A260" t="s">
         <v>122</v>
       </c>
@@ -5419,7 +5599,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="261" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:3">
       <c r="A261" t="s">
         <v>116</v>
       </c>
@@ -5427,10 +5607,10 @@
         <v>553</v>
       </c>
       <c r="C261" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.2">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3">
       <c r="A262" t="s">
         <v>127</v>
       </c>
@@ -5441,7 +5621,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="263" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:3">
       <c r="A263" t="s">
         <v>555</v>
       </c>
@@ -5452,7 +5632,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="264" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:3">
       <c r="A264" t="s">
         <v>556</v>
       </c>
@@ -5463,10 +5643,275 @@
         <v>557</v>
       </c>
     </row>
+    <row r="265" spans="1:3">
+      <c r="A265" t="s">
+        <v>563</v>
+      </c>
+      <c r="B265" t="s">
+        <v>568</v>
+      </c>
+      <c r="C265" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3">
+      <c r="A266" t="s">
+        <v>564</v>
+      </c>
+      <c r="B266" t="s">
+        <v>568</v>
+      </c>
+      <c r="C266" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3">
+      <c r="A267" t="s">
+        <v>565</v>
+      </c>
+      <c r="B267" t="s">
+        <v>568</v>
+      </c>
+      <c r="C267" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3">
+      <c r="A268" t="s">
+        <v>566</v>
+      </c>
+      <c r="B268" t="s">
+        <v>569</v>
+      </c>
+      <c r="C268" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3">
+      <c r="A269" t="s">
+        <v>567</v>
+      </c>
+      <c r="B269" t="s">
+        <v>569</v>
+      </c>
+      <c r="C269" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3">
+      <c r="A270" t="s">
+        <v>562</v>
+      </c>
+      <c r="B270" t="s">
+        <v>569</v>
+      </c>
+      <c r="C270" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3">
+      <c r="A271" t="s">
+        <v>570</v>
+      </c>
+      <c r="B271" t="s">
+        <v>571</v>
+      </c>
+      <c r="C271" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3">
+      <c r="A272" t="s">
+        <v>575</v>
+      </c>
+      <c r="B272" t="s">
+        <v>572</v>
+      </c>
+      <c r="C272" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3">
+      <c r="A273" t="s">
+        <v>576</v>
+      </c>
+      <c r="B273" t="s">
+        <v>573</v>
+      </c>
+      <c r="C273" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3">
+      <c r="A274" t="s">
+        <v>577</v>
+      </c>
+      <c r="B274" t="s">
+        <v>574</v>
+      </c>
+      <c r="C274" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3">
+      <c r="A275" t="s">
+        <v>579</v>
+      </c>
+      <c r="B275" t="s">
+        <v>587</v>
+      </c>
+      <c r="C275" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3">
+      <c r="A276" t="s">
+        <v>580</v>
+      </c>
+      <c r="B276" t="s">
+        <v>587</v>
+      </c>
+      <c r="C276" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3">
+      <c r="A277" t="s">
+        <v>581</v>
+      </c>
+      <c r="B277" t="s">
+        <v>587</v>
+      </c>
+      <c r="C277" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3">
+      <c r="A278" t="s">
+        <v>582</v>
+      </c>
+      <c r="B278" t="s">
+        <v>587</v>
+      </c>
+      <c r="C278" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3">
+      <c r="A279" t="s">
+        <v>583</v>
+      </c>
+      <c r="B279" t="s">
+        <v>587</v>
+      </c>
+      <c r="C279" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3">
+      <c r="A280" t="s">
+        <v>584</v>
+      </c>
+      <c r="B280" t="s">
+        <v>587</v>
+      </c>
+      <c r="C280" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3">
+      <c r="A281" t="s">
+        <v>585</v>
+      </c>
+      <c r="B281" t="s">
+        <v>587</v>
+      </c>
+      <c r="C281" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="282" spans="1:3">
+      <c r="A282" t="s">
+        <v>586</v>
+      </c>
+      <c r="B282" t="s">
+        <v>587</v>
+      </c>
+      <c r="C282" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="283" spans="1:3">
+      <c r="A283" t="s">
+        <v>589</v>
+      </c>
+      <c r="B283" t="s">
+        <v>595</v>
+      </c>
+      <c r="C283" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="284" spans="1:3">
+      <c r="A284" t="s">
+        <v>590</v>
+      </c>
+      <c r="B284" t="s">
+        <v>595</v>
+      </c>
+      <c r="C284" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="285" spans="1:3">
+      <c r="A285" t="s">
+        <v>591</v>
+      </c>
+      <c r="B285" t="s">
+        <v>595</v>
+      </c>
+      <c r="C285" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="286" spans="1:3">
+      <c r="A286" t="s">
+        <v>592</v>
+      </c>
+      <c r="B286" t="s">
+        <v>595</v>
+      </c>
+      <c r="C286" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="287" spans="1:3">
+      <c r="A287" t="s">
+        <v>593</v>
+      </c>
+      <c r="B287" t="s">
+        <v>595</v>
+      </c>
+      <c r="C287" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="288" spans="1:3">
+      <c r="A288" t="s">
+        <v>594</v>
+      </c>
+      <c r="B288" t="s">
+        <v>595</v>
+      </c>
+      <c r="C288" t="s">
+        <v>596</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A1:A275">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A274">
     <sortCondition ref="A1"/>
   </sortState>
+  <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>